<commit_message>
new file:   Sine/.vscode/settings.json 	new file:   Sine/a.exe 	modified:   Sine/main.c 	modified:   Sine/reference/cordic map.xlsx 	new file:   Sine/reference/~$cordic map.xlsx 	modified:   Sine/sine.c
</commit_message>
<xml_diff>
--- a/Sine/reference/cordic map.xlsx
+++ b/Sine/reference/cordic map.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding Files\C n Cpp\CORDIC\reference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys32\home\Vidda\C\Sine\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AAB3A8-0A1B-4C7B-9D84-10DE325A7C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC970DB2-2211-4C66-82DB-AE3BE6167F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2355" windowWidth="20730" windowHeight="11160" xr2:uid="{EE51D47B-CF80-4A69-8C4A-2314D6D3AEEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EE51D47B-CF80-4A69-8C4A-2314D6D3AEEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Cordic calc" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>a</t>
   </si>
@@ -81,6 +82,72 @@
   </si>
   <si>
     <t>Sine</t>
+  </si>
+  <si>
+    <t>Iterations</t>
+  </si>
+  <si>
+    <t>tan(deg)</t>
+  </si>
+  <si>
+    <t>cos(deg)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Angle (deg)</t>
+  </si>
+  <si>
+    <t>Curr Angle</t>
+  </si>
+  <si>
+    <t>Using Real Angles</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Fx Point</t>
+  </si>
+  <si>
+    <t>Using Fixed Point Representation, 8 bits fractional</t>
+  </si>
+  <si>
+    <t># Fractional bits</t>
+  </si>
+  <si>
+    <t>Fraction</t>
+  </si>
+  <si>
+    <t>0x8001</t>
+  </si>
+  <si>
+    <t>0x4380</t>
+  </si>
+  <si>
+    <t>0x2D00</t>
+  </si>
+  <si>
+    <t>0xE001</t>
+  </si>
+  <si>
+    <t>0x3840</t>
+  </si>
+  <si>
+    <t>0x4801</t>
+  </si>
+  <si>
+    <t>0x32A0</t>
+  </si>
+  <si>
+    <t>D8A3</t>
+  </si>
+  <si>
+    <t>3BE0</t>
   </si>
 </sst>
 </file>
@@ -116,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -126,6 +193,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8948,6 +9018,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>60857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDCAC322-162A-E5C6-7396-649BC146A8AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1952625" y="4838700"/>
+          <a:ext cx="5972175" cy="3413657"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9247,8 +9366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1ABA728-31A9-4078-B10B-6F229B57FA1A}">
   <dimension ref="A2:JJ260"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView topLeftCell="C217" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54:J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15562,7 +15681,7 @@
   <dimension ref="C4:IX5"/>
   <sheetViews>
     <sheetView topLeftCell="GQ1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:IX4"/>
+      <selection activeCell="HO14" sqref="HO14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17369,4 +17488,1304 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1FE35D-41D3-41FF-8C16-1DF9B89A1C0D}">
+  <dimension ref="G1:AR25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="11.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="Q1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="AA1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AK1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="1">
+        <v>55</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>12800</v>
+      </c>
+      <c r="AC2" s="1"/>
+      <c r="AK2">
+        <v>8</v>
+      </c>
+      <c r="AL2">
+        <v>90</v>
+      </c>
+      <c r="AM2">
+        <f>_xlfn.BITLSHIFT(AL2,AK2)</f>
+        <v>23040</v>
+      </c>
+      <c r="AO2">
+        <v>0.60725300000000004</v>
+      </c>
+      <c r="AP2">
+        <f>AO2*2^AK2</f>
+        <v>155.45676800000001</v>
+      </c>
+      <c r="AQ2">
+        <f>AM2*AP2</f>
+        <v>3581723.9347200003</v>
+      </c>
+      <c r="AR2" t="e">
+        <f>_xlfn.BITRSHIFT(AQ2,16)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="3" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <f>COS(RADIANS(H2))</f>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="I3" s="1">
+        <f>SIN(RADIANS(H2))</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="R3" s="1">
+        <f>COS(RADIANS(R2))</f>
+        <v>0.57357643635104616</v>
+      </c>
+      <c r="S3" s="1">
+        <f>SIN(RADIANS(R2))</f>
+        <v>0.8191520442889918</v>
+      </c>
+      <c r="AB3" s="1">
+        <f>COS(RADIANS(AB2))</f>
+        <v>-0.93969262078591032</v>
+      </c>
+      <c r="AC3" s="1">
+        <f>SIN(RADIANS(AB2))</f>
+        <v>-0.34202014332566349</v>
+      </c>
+      <c r="AM3">
+        <f>2^AK2</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>45</v>
+      </c>
+      <c r="K5" s="1">
+        <v>45</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L10" si="0">TAN(RADIANS(J5))</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M11" si="1">COS(RADIANS(J5))</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>256</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>45</v>
+      </c>
+      <c r="U5" s="1">
+        <v>45</v>
+      </c>
+      <c r="V5">
+        <f>2^Q5</f>
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ref="W5:W11" si="2">COS(RADIANS(T5))</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ref="X5:X11" si="3">2^-Q5</f>
+        <v>1</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>256</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>11520</v>
+      </c>
+      <c r="AE5">
+        <v>11520</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" ref="AF5:AF10" si="4">TAN(RADIANS(AD5))</f>
+        <v>-7.8409501114151681E-15</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" ref="AG5:AG11" si="5">COS(RADIANS(AD5))</f>
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <f>55459/2^AK2</f>
+        <v>216.63671875</v>
+      </c>
+    </row>
+    <row r="6" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <f>H5-I5*L5</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <f>I5+H5*L5</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J10" si="6">IF($H$2&gt;K5,ABS(J5/2),-ABS(J5/2))</f>
+        <v>22.5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K10" si="7">J6+K5</f>
+        <v>67.5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.41421356237309503</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>0.92387953251128674</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" ref="R6:R10" si="8">R5+IF(T5&gt;0,-S5*V5,S5*V5)</f>
+        <v>256</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" ref="S6:S10" si="9">S5+IF(T5&gt;0,R5*V5,-R5*V5)</f>
+        <v>256</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6:T10" si="10">IF($R$2&gt;U5,ABS(T5/2),-ABS(T5/2))</f>
+        <v>22.5</v>
+      </c>
+      <c r="U6">
+        <f t="shared" ref="U6:U10" si="11">T6+U5</f>
+        <v>67.5</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6:V10" si="12">2^-Q6</f>
+        <v>0.5</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="2"/>
+        <v>0.92387953251128674</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="1">
+        <f t="shared" ref="AB6:AB10" si="13">AB5+IF($AB$2&gt;AE5,-_xlfn.BITRSHIFT(AC5,AA5),_xlfn.BITRSHIFT(AC5,AA5))</f>
+        <v>256</v>
+      </c>
+      <c r="AC6" s="1">
+        <f>AC5+IF($AB$2&gt;AE5,_xlfn.BITRSHIFT(AB5,AA5),-_xlfn.BITRSHIFT(AB5,AA5))</f>
+        <v>256</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" ref="AD6:AD10" si="14">IF($AB$2&gt;AE5,ABS(AD5/2),-ABS(AD5/2))</f>
+        <v>5760</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6:AE10" si="15">AD6+AE5</f>
+        <v>17280</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="4"/>
+        <v>-3.920475055707584E-15</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1">
+        <f>H6-I6*L6</f>
+        <v>0.58578643762690508</v>
+      </c>
+      <c r="I7" s="1">
+        <f>I6+H6*L6</f>
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="6"/>
+        <v>-11.25</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="7"/>
+        <v>56.25</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>-0.19891236737965801</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.98078528040323043</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>2</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="8"/>
+        <v>128</v>
+      </c>
+      <c r="S7" s="1">
+        <f t="shared" si="9"/>
+        <v>384</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="10"/>
+        <v>-11.25</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="11"/>
+        <v>56.25</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="12"/>
+        <v>0.25</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="2"/>
+        <v>0.98078528040323043</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="1">
+        <f t="shared" si="13"/>
+        <v>384</v>
+      </c>
+      <c r="AC7" s="1">
+        <f>AC6+IF($AB$2&gt;AE6,-_xlfn.BITRSHIFT(AB6,AA6),_xlfn.BITRSHIFT(AB6,AA6))</f>
+        <v>384</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="14"/>
+        <v>-2880</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="15"/>
+        <v>14400</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="4"/>
+        <v>1.960237527853792E-15</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <f>H7-I7*L7</f>
+        <v>0.86709100529895711</v>
+      </c>
+      <c r="I8" s="1">
+        <f>I7+H7*L7</f>
+        <v>1.2976933952858309</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="6"/>
+        <v>5.625</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="7"/>
+        <v>61.875</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>9.8491403357164248E-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.99518472667219693</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>3</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="8"/>
+        <v>224</v>
+      </c>
+      <c r="S8" s="1">
+        <f t="shared" si="9"/>
+        <v>352</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="10"/>
+        <v>-5.625</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="11"/>
+        <v>50.625</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="12"/>
+        <v>0.125</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="2"/>
+        <v>0.99518472667219693</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="1">
+        <f t="shared" si="13"/>
+        <v>480</v>
+      </c>
+      <c r="AC8" s="1">
+        <f>AC7+IF($AB$2&gt;AE7,-_xlfn.BITRSHIFT(AB7,AA7),_xlfn.BITRSHIFT(AB7,AA7))</f>
+        <v>480</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="14"/>
+        <v>-1440</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="15"/>
+        <v>12960</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="4"/>
+        <v>9.8011876392689601E-16</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AM8">
+        <v>727</v>
+      </c>
+      <c r="AN8">
+        <f>AM8/2048</f>
+        <v>0.35498046875</v>
+      </c>
+    </row>
+    <row r="9" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <f>H8-I8*L8</f>
+        <v>0.73927936166993236</v>
+      </c>
+      <c r="I9" s="1">
+        <f>I8+H8*L8</f>
+        <v>1.3830944052360996</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="6"/>
+        <v>-2.8125</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="7"/>
+        <v>59.0625</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>-4.9126849769467254E-2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>0.99879545620517241</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>4</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="8"/>
+        <v>268</v>
+      </c>
+      <c r="S9" s="1">
+        <f t="shared" si="9"/>
+        <v>324</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="10"/>
+        <v>2.8125</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="11"/>
+        <v>53.4375</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="12"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="2"/>
+        <v>0.99879545620517241</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="3"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB9" s="1">
+        <f t="shared" si="13"/>
+        <v>540</v>
+      </c>
+      <c r="AC9" s="1">
+        <f>AC8+IF($AB$2&gt;AE8,-_xlfn.BITRSHIFT(AB8,AA8),_xlfn.BITRSHIFT(AB8,AA8))</f>
+        <v>540</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="14"/>
+        <v>-720</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="15"/>
+        <v>12240</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="4"/>
+        <v>4.90059381963448E-16</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <v>1594</v>
+      </c>
+      <c r="AN9">
+        <f>AM9/2048</f>
+        <v>0.7783203125</v>
+      </c>
+    </row>
+    <row r="10" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1">
+        <f>H9-I9*L9</f>
+        <v>0.80722643273295691</v>
+      </c>
+      <c r="I10" s="1">
+        <f>I9+H9*L9</f>
+        <v>1.3467759390976732</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>1.40625</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="7"/>
+        <v>60.46875</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2.4548622108925444E-2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>0.99969881869620425</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>5</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="8"/>
+        <v>247.75</v>
+      </c>
+      <c r="S10" s="1">
+        <f t="shared" si="9"/>
+        <v>340.75</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="10"/>
+        <v>1.40625</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="11"/>
+        <v>54.84375</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="12"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="2"/>
+        <v>0.99969881869620425</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="3"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB10" s="1">
+        <f t="shared" si="13"/>
+        <v>507</v>
+      </c>
+      <c r="AC10" s="1">
+        <f>AC9+IF($AB$2&gt;AE9,-_xlfn.BITRSHIFT(AB9,AA9),_xlfn.BITRSHIFT(AB9,AA9))</f>
+        <v>507</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="14"/>
+        <v>360</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="15"/>
+        <v>12600</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="4"/>
+        <v>-2.45029690981724E-16</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <f>H10*M11</f>
+        <v>0.51394790605844076</v>
+      </c>
+      <c r="I11" s="1">
+        <f>I10*M11</f>
+        <v>0.85747027817920929</v>
+      </c>
+      <c r="M11">
+        <f>PRODUCT(M5:M10)</f>
+        <v>0.63668369272598235</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>6</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" ref="R11:R17" si="16">R10+IF(T10&gt;0,-S10*V10,S10*V10)</f>
+        <v>237.1015625</v>
+      </c>
+      <c r="S11" s="1">
+        <f t="shared" ref="S11:S17" si="17">S10+IF(T10&gt;0,R10*V10,-R10*V10)</f>
+        <v>348.4921875</v>
+      </c>
+      <c r="T11">
+        <f t="shared" ref="T11:T17" si="18">IF($R$2&gt;U10,ABS(T10/2),-ABS(T10/2))</f>
+        <v>0.703125</v>
+      </c>
+      <c r="U11">
+        <f t="shared" ref="U11:U17" si="19">T11+U10</f>
+        <v>55.546875</v>
+      </c>
+      <c r="V11">
+        <f t="shared" ref="V11:V17" si="20">2^-Q11</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="W11">
+        <f t="shared" ref="W11:W17" si="21">COS(RADIANS(T11))</f>
+        <v>0.9999247018391445</v>
+      </c>
+      <c r="X11">
+        <f t="shared" ref="X11:X17" si="22">2^-Q11</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11">
+        <f>SUM(AD5:AD10)</f>
+        <v>12600</v>
+      </c>
+    </row>
+    <row r="12" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="H12" s="1">
+        <f>H11^2</f>
+        <v>0.26414245014185583</v>
+      </c>
+      <c r="I12" s="1">
+        <f>I11^2</f>
+        <v>0.73525527796073054</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>7</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="16"/>
+        <v>231.6563720703125</v>
+      </c>
+      <c r="S12" s="1">
+        <f t="shared" si="17"/>
+        <v>352.1968994140625</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="18"/>
+        <v>-0.3515625</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="19"/>
+        <v>55.1953125</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="20"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="21"/>
+        <v>0.99998117528260111</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="22"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="AB12" s="1"/>
+      <c r="AK12">
+        <f>1594^2</f>
+        <v>2540836</v>
+      </c>
+    </row>
+    <row r="13" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="H13" s="1">
+        <f>SQRT(H12+I12)</f>
+        <v>0.99969881869620425</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>8</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="16"/>
+        <v>234.40791034698486</v>
+      </c>
+      <c r="S13" s="1">
+        <f t="shared" si="17"/>
+        <v>350.38708400726318</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="18"/>
+        <v>-0.17578125</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="19"/>
+        <v>55.01953125</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="20"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="21"/>
+        <v>0.99999529380957619</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="22"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="AK13">
+        <f>727^2</f>
+        <v>528529</v>
+      </c>
+    </row>
+    <row r="14" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1">
+        <v>9</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="16"/>
+        <v>235.77660989388824</v>
+      </c>
+      <c r="S14" s="1">
+        <f t="shared" si="17"/>
+        <v>349.47142810747027</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="18"/>
+        <v>-8.7890625E-2</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="19"/>
+        <v>54.931640625</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="20"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="21"/>
+        <v>0.99999882345170188</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="22"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="AK14">
+        <f>SQRT(AK12+AK13)</f>
+        <v>1751.960330601124</v>
+      </c>
+    </row>
+    <row r="15" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1">
+        <v>10</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="16"/>
+        <v>236.45917127691064</v>
+      </c>
+      <c r="S15" s="1">
+        <f t="shared" si="17"/>
+        <v>349.01092691627127</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="18"/>
+        <v>4.39453125E-2</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="19"/>
+        <v>54.9755859375</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="20"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="21"/>
+        <v>0.99999970586288223</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="22"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>1</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="7:44" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1">
+        <v>11</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="16"/>
+        <v>236.11834029359397</v>
+      </c>
+      <c r="S16" s="1">
+        <f t="shared" si="17"/>
+        <v>349.24184407572136</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="18"/>
+        <v>2.197265625E-2</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="19"/>
+        <v>54.99755859375</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="20"/>
+        <v>4.8828125E-4</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="21"/>
+        <v>0.99999992646571789</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="22"/>
+        <v>4.8828125E-4</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>11520</v>
+      </c>
+      <c r="AE16">
+        <v>1</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
+        <v>115200</v>
+      </c>
+    </row>
+    <row r="17" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="H17" s="1">
+        <v>142</v>
+      </c>
+      <c r="I17" s="1">
+        <v>211</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>12</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="16"/>
+        <v>235.94781204941637</v>
+      </c>
+      <c r="S17" s="1">
+        <f t="shared" si="17"/>
+        <v>349.35713623406787</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="18"/>
+        <v>1.0986328125E-2</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="19"/>
+        <v>55.008544921875</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="20"/>
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="21"/>
+        <v>0.99999998161642933</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="22"/>
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="AB17">
+        <v>-66355199</v>
+      </c>
+      <c r="AC17">
+        <v>17280</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH17">
+        <v>-32767</v>
+      </c>
+      <c r="AI17">
+        <v>17280</v>
+      </c>
+    </row>
+    <row r="18" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="H18" s="1">
+        <f>H17^2</f>
+        <v>20164</v>
+      </c>
+      <c r="I18" s="1">
+        <f>I17^2</f>
+        <v>44521</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>13</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" ref="R18:R20" si="23">R17+IF(T17&gt;0,-S17*V17,S17*V17)</f>
+        <v>235.86251977982798</v>
+      </c>
+      <c r="S18" s="1">
+        <f t="shared" ref="S18:S20" si="24">S17+IF(T17&gt;0,R17*V17,-R17*V17)</f>
+        <v>349.41474068036899</v>
+      </c>
+      <c r="T18">
+        <f t="shared" ref="T18:T20" si="25">IF($R$2&gt;U17,ABS(T17/2),-ABS(T17/2))</f>
+        <v>-5.4931640625E-3</v>
+      </c>
+      <c r="U18">
+        <f t="shared" ref="U18:U20" si="26">T18+U17</f>
+        <v>55.0030517578125</v>
+      </c>
+      <c r="V18">
+        <f t="shared" ref="V18:V20" si="27">2^-Q18</f>
+        <v>1.220703125E-4</v>
+      </c>
+      <c r="W18">
+        <f t="shared" ref="W18:W21" si="28">COS(RADIANS(T18))</f>
+        <v>0.99999999540410733</v>
+      </c>
+      <c r="X18">
+        <f t="shared" ref="X18:X20" si="29">2^-Q18</f>
+        <v>1.220703125E-4</v>
+      </c>
+      <c r="AB18">
+        <v>-16588799</v>
+      </c>
+      <c r="AC18">
+        <v>191102990400</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH18">
+        <v>-8191</v>
+      </c>
+      <c r="AI18">
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="19" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="H19" s="1">
+        <f>SQRT(H18+I18)</f>
+        <v>254.33245958783948</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>14</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="23"/>
+        <v>235.90517294641495</v>
+      </c>
+      <c r="S19" s="1">
+        <f t="shared" si="24"/>
+        <v>349.38594886887245</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="25"/>
+        <v>-2.74658203125E-3</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="26"/>
+        <v>55.00030517578125</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="27"/>
+        <v>6.103515625E-5</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="28"/>
+        <v>0.99999999885102686</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="29"/>
+        <v>6.103515625E-5</v>
+      </c>
+      <c r="AB19">
+        <v>275188289587201</v>
+      </c>
+      <c r="AC19">
+        <v>214990860960</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH19">
+        <v>18433</v>
+      </c>
+      <c r="AI19">
+        <v>12960</v>
+      </c>
+    </row>
+    <row r="20" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="Q20" s="1">
+        <v>15</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="23"/>
+        <v>235.92649777239572</v>
+      </c>
+      <c r="S20" s="1">
+        <f t="shared" si="24"/>
+        <v>349.37155035978145</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="25"/>
+        <v>-1.373291015625E-3</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="26"/>
+        <v>54.998931884765625</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="27"/>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="28"/>
+        <v>0.99999999971275666</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="29"/>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="AB20">
+        <v>429981709478401</v>
+      </c>
+      <c r="AC20">
+        <v>-1.9813535351192374E+17</v>
+      </c>
+    </row>
+    <row r="21" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="R21" s="1">
+        <f>R20*T21</f>
+        <v>36568.607154721336</v>
+      </c>
+      <c r="S21" s="1">
+        <f>S20*T21</f>
+        <v>54152.590305766127</v>
+      </c>
+      <c r="T21">
+        <v>155</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="28"/>
+        <v>-0.90630778703664994</v>
+      </c>
+      <c r="AB21">
+        <v>7.132915724600202E+19</v>
+      </c>
+      <c r="AC21">
+        <v>-4.3341938099699392E+16</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="R22" s="1">
+        <f>ROUND(R21,0)</f>
+        <v>36569</v>
+      </c>
+      <c r="S22" s="1">
+        <f>ROUND(S21,0)</f>
+        <v>54153</v>
+      </c>
+    </row>
+    <row r="23" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="R23" s="1">
+        <f>_xlfn.BITRSHIFT(R22,8)</f>
+        <v>142</v>
+      </c>
+      <c r="S23" s="1">
+        <f>_xlfn.BITRSHIFT(S22,8)</f>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="R24" s="1">
+        <f>R23^2</f>
+        <v>20164</v>
+      </c>
+      <c r="S24" s="1">
+        <f>S23^2</f>
+        <v>44521</v>
+      </c>
+    </row>
+    <row r="25" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="R25" s="1">
+        <f>SQRT(R24+S24)</f>
+        <v>254.33245958783948</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G1:M1"/>
+    <mergeCell ref="AA1:AG1"/>
+    <mergeCell ref="Q1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new file:   Inverse_Kinematics/inv_kine.c 	new file:   Inverse_Kinematics/inv_kine.h 	new file:   Inverse_Kinematics/main.c 	modified:   Sine/.vscode/settings.json 	modified:   Sine/a.exe 	modified:   Sine/main.c 	modified:   Sine/reference/cordic map.xlsx 	modified:   Sine/sine.c 	modified:   Sine/sine.h
</commit_message>
<xml_diff>
--- a/Sine/reference/cordic map.xlsx
+++ b/Sine/reference/cordic map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys32\home\Vidda\C\Sine\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC970DB2-2211-4C66-82DB-AE3BE6167F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AADA79E-BF8A-41D1-B7BB-412FD417A6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EE51D47B-CF80-4A69-8C4A-2314D6D3AEEC}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="22">
   <si>
     <t>a</t>
   </si>
@@ -114,40 +114,16 @@
     <t>Fx Point</t>
   </si>
   <si>
-    <t>Using Fixed Point Representation, 8 bits fractional</t>
-  </si>
-  <si>
     <t># Fractional bits</t>
   </si>
   <si>
     <t>Fraction</t>
   </si>
   <si>
-    <t>0x8001</t>
+    <t>Unit Vector In Fixed Point</t>
   </si>
   <si>
-    <t>0x4380</t>
-  </si>
-  <si>
-    <t>0x2D00</t>
-  </si>
-  <si>
-    <t>0xE001</t>
-  </si>
-  <si>
-    <t>0x3840</t>
-  </si>
-  <si>
-    <t>0x4801</t>
-  </si>
-  <si>
-    <t>0x32A0</t>
-  </si>
-  <si>
-    <t>D8A3</t>
-  </si>
-  <si>
-    <t>3BE0</t>
+    <t>Unit Vector and Angle In Fixed Point</t>
   </si>
 </sst>
 </file>
@@ -17492,10 +17468,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1FE35D-41D3-41FF-8C16-1DF9B89A1C0D}">
-  <dimension ref="G1:AR25"/>
+  <dimension ref="G1:AR55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17509,7 +17485,11 @@
     <col min="19" max="19" width="11.28515625" style="1" customWidth="1"/>
     <col min="21" max="21" width="12.42578125" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.85546875" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="1"/>
+    <col min="30" max="30" width="11.28515625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="12.42578125" customWidth="1"/>
+    <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17524,7 +17504,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="Q1" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
@@ -17532,17 +17512,17 @@
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
-      <c r="AA1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB1" s="4"/>
+      <c r="AB1" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
       <c r="AK1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AL1" t="s">
         <v>16</v>
@@ -17551,7 +17531,7 @@
         <v>17</v>
       </c>
       <c r="AO1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AP1" t="s">
         <v>17</v>
@@ -17568,24 +17548,24 @@
         <v>13</v>
       </c>
       <c r="R2" s="1">
-        <v>55</v>
-      </c>
-      <c r="AA2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="1">
-        <v>12800</v>
-      </c>
-      <c r="AC2" s="1"/>
+      <c r="AC2" s="1">
+        <f>ROUND(AM2,0)</f>
+        <v>11520</v>
+      </c>
       <c r="AK2">
         <v>8</v>
       </c>
       <c r="AL2">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="AM2">
-        <f>_xlfn.BITLSHIFT(AL2,AK2)</f>
-        <v>23040</v>
+        <f>AL2*2^AK2</f>
+        <v>11520</v>
       </c>
       <c r="AO2">
         <v>0.60725300000000004</v>
@@ -17596,7 +17576,7 @@
       </c>
       <c r="AQ2">
         <f>AM2*AP2</f>
-        <v>3581723.9347200003</v>
+        <v>1790861.9673600001</v>
       </c>
       <c r="AR2" t="e">
         <f>_xlfn.BITRSHIFT(AQ2,16)</f>
@@ -17614,19 +17594,23 @@
       </c>
       <c r="R3" s="1">
         <f>COS(RADIANS(R2))</f>
-        <v>0.57357643635104616</v>
+        <v>0.64278760968653936</v>
       </c>
       <c r="S3" s="1">
         <f>SIN(RADIANS(R2))</f>
-        <v>0.8191520442889918</v>
-      </c>
-      <c r="AB3" s="1">
-        <f>COS(RADIANS(AB2))</f>
-        <v>-0.93969262078591032</v>
+        <v>0.76604444311897801</v>
       </c>
       <c r="AC3" s="1">
-        <f>SIN(RADIANS(AB2))</f>
-        <v>-0.34202014332566349</v>
+        <f>COS(RADIANS(AL2))</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="AD3" s="1">
+        <f>SIN(RADIANS(AL2))</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="AL3">
+        <f>AM2*1.5</f>
+        <v>17280</v>
       </c>
       <c r="AM3">
         <f>2^AK2</f>
@@ -17676,26 +17660,35 @@
       <c r="W4" t="s">
         <v>10</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>9</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>10</v>
+      </c>
+      <c r="AK4">
+        <f>45*256</f>
+        <v>11520</v>
+      </c>
+      <c r="AM4" t="str">
+        <f>DEC2HEX(AM2)</f>
+        <v>2D00</v>
       </c>
     </row>
     <row r="5" spans="7:44" x14ac:dyDescent="0.25">
@@ -17719,14 +17712,14 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M11" si="1">COS(RADIANS(J5))</f>
+        <f t="shared" ref="M5:M10" si="1">COS(RADIANS(J5))</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="Q5" s="1">
         <v>0</v>
       </c>
       <c r="R5" s="1">
-        <v>256</v>
+        <v>2048</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
@@ -17742,34 +17735,39 @@
         <v>1</v>
       </c>
       <c r="W5">
-        <f t="shared" ref="W5:W11" si="2">COS(RADIANS(T5))</f>
+        <f t="shared" ref="W5:W10" si="2">COS(RADIANS(T5))</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="X5">
-        <f t="shared" ref="X5:X11" si="3">2^-Q5</f>
+        <f t="shared" ref="X5:X10" si="3">2^-Q5</f>
         <v>1</v>
       </c>
-      <c r="AA5" s="1">
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1">
         <v>0</v>
       </c>
-      <c r="AB5" s="1">
-        <v>256</v>
-      </c>
       <c r="AC5" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AD5" s="1">
         <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>11520</v>
       </c>
       <c r="AE5">
         <v>11520</v>
       </c>
       <c r="AF5">
-        <f t="shared" ref="AF5:AF10" si="4">TAN(RADIANS(AD5))</f>
-        <v>-7.8409501114151681E-15</v>
+        <v>11520</v>
       </c>
       <c r="AG5">
-        <f t="shared" ref="AG5:AG11" si="5">COS(RADIANS(AD5))</f>
+        <f>2^AB5</f>
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" ref="AH5:AH21" si="4">COS(RADIANS(AE5))</f>
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" ref="AI5:AI20" si="5">2^-AB5</f>
         <v>1</v>
       </c>
       <c r="AL5">
@@ -17810,11 +17808,11 @@
       </c>
       <c r="R6" s="1">
         <f t="shared" ref="R6:R10" si="8">R5+IF(T5&gt;0,-S5*V5,S5*V5)</f>
-        <v>256</v>
+        <v>2048</v>
       </c>
       <c r="S6" s="1">
         <f t="shared" ref="S6:S10" si="9">S5+IF(T5&gt;0,R5*V5,-R5*V5)</f>
-        <v>256</v>
+        <v>2048</v>
       </c>
       <c r="T6">
         <f t="shared" ref="T6:T10" si="10">IF($R$2&gt;U5,ABS(T5/2),-ABS(T5/2))</f>
@@ -17836,32 +17834,37 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1">
         <v>1</v>
       </c>
-      <c r="AB6" s="1">
-        <f t="shared" ref="AB6:AB10" si="13">AB5+IF($AB$2&gt;AE5,-_xlfn.BITRSHIFT(AC5,AA5),_xlfn.BITRSHIFT(AC5,AA5))</f>
-        <v>256</v>
-      </c>
       <c r="AC6" s="1">
-        <f>AC5+IF($AB$2&gt;AE5,_xlfn.BITRSHIFT(AB5,AA5),-_xlfn.BITRSHIFT(AB5,AA5))</f>
-        <v>256</v>
-      </c>
-      <c r="AD6">
-        <f t="shared" ref="AD6:AD10" si="14">IF($AB$2&gt;AE5,ABS(AD5/2),-ABS(AD5/2))</f>
+        <f t="shared" ref="AC6:AC20" si="13">AC5+IF(AE5&gt;0,-_xlfn.BITRSHIFT(AD5,AB5),_xlfn.BITRSHIFT(AD5,AB5))</f>
+        <v>2048</v>
+      </c>
+      <c r="AD6" s="1">
+        <f t="shared" ref="AD6:AD20" si="14">AD5+IF(AE5&gt;0,_xlfn.BITRSHIFT(AC5,AB5),-_xlfn.BITRSHIFT(AC5,AB5))</f>
+        <v>2048</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" ref="AE6:AE20" si="15">IF($AC$2&gt;AF5,ABS(AE5/2),-ABS(AE5/2))</f>
+        <v>-5760</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" ref="AF6:AF20" si="16">AE6+AF5</f>
         <v>5760</v>
       </c>
-      <c r="AE6">
-        <f t="shared" ref="AE6:AE10" si="15">AD6+AE5</f>
-        <v>17280</v>
-      </c>
-      <c r="AF6">
+      <c r="AG6">
+        <f t="shared" ref="AG6:AG20" si="17">2^-AB6</f>
+        <v>0.5</v>
+      </c>
+      <c r="AH6">
         <f t="shared" si="4"/>
-        <v>-3.920475055707584E-15</v>
-      </c>
-      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="7:44" x14ac:dyDescent="0.25">
@@ -17897,11 +17900,11 @@
       </c>
       <c r="R7" s="1">
         <f t="shared" si="8"/>
-        <v>128</v>
+        <v>1024</v>
       </c>
       <c r="S7" s="1">
         <f t="shared" si="9"/>
-        <v>384</v>
+        <v>3072</v>
       </c>
       <c r="T7">
         <f t="shared" si="10"/>
@@ -17923,32 +17926,41 @@
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1">
         <v>2</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AC7" s="1">
         <f t="shared" si="13"/>
-        <v>384</v>
-      </c>
-      <c r="AC7" s="1">
-        <f>AC6+IF($AB$2&gt;AE6,-_xlfn.BITRSHIFT(AB6,AA6),_xlfn.BITRSHIFT(AB6,AA6))</f>
-        <v>384</v>
-      </c>
-      <c r="AD7">
+        <v>3072</v>
+      </c>
+      <c r="AD7" s="1">
         <f t="shared" si="14"/>
-        <v>-2880</v>
+        <v>1024</v>
       </c>
       <c r="AE7">
         <f t="shared" si="15"/>
-        <v>14400</v>
+        <v>2880</v>
       </c>
       <c r="AF7">
+        <f t="shared" si="16"/>
+        <v>8640</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="17"/>
+        <v>0.25</v>
+      </c>
+      <c r="AH7">
         <f t="shared" si="4"/>
-        <v>1.960237527853792E-15</v>
-      </c>
-      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.25</v>
+      </c>
+      <c r="AK7">
+        <f>45*4096</f>
+        <v>184320</v>
       </c>
     </row>
     <row r="8" spans="7:44" x14ac:dyDescent="0.25">
@@ -17984,11 +17996,11 @@
       </c>
       <c r="R8" s="1">
         <f t="shared" si="8"/>
-        <v>224</v>
+        <v>1792</v>
       </c>
       <c r="S8" s="1">
         <f t="shared" si="9"/>
-        <v>352</v>
+        <v>2816</v>
       </c>
       <c r="T8">
         <f t="shared" si="10"/>
@@ -18010,32 +18022,37 @@
         <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1">
         <v>3</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AC8" s="1">
         <f t="shared" si="13"/>
-        <v>480</v>
-      </c>
-      <c r="AC8" s="1">
-        <f>AC7+IF($AB$2&gt;AE7,-_xlfn.BITRSHIFT(AB7,AA7),_xlfn.BITRSHIFT(AB7,AA7))</f>
-        <v>480</v>
-      </c>
-      <c r="AD8">
+        <v>2816</v>
+      </c>
+      <c r="AD8" s="1">
         <f t="shared" si="14"/>
-        <v>-1440</v>
+        <v>1792</v>
       </c>
       <c r="AE8">
         <f t="shared" si="15"/>
-        <v>12960</v>
+        <v>1440</v>
       </c>
       <c r="AF8">
+        <f t="shared" si="16"/>
+        <v>10080</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="17"/>
+        <v>0.125</v>
+      </c>
+      <c r="AH8">
         <f t="shared" si="4"/>
-        <v>9.8011876392689601E-16</v>
-      </c>
-      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.125</v>
       </c>
       <c r="AM8">
         <v>727</v>
@@ -18078,19 +18095,19 @@
       </c>
       <c r="R9" s="1">
         <f t="shared" si="8"/>
-        <v>268</v>
+        <v>2144</v>
       </c>
       <c r="S9" s="1">
         <f t="shared" si="9"/>
-        <v>324</v>
+        <v>2592</v>
       </c>
       <c r="T9">
         <f t="shared" si="10"/>
-        <v>2.8125</v>
+        <v>-2.8125</v>
       </c>
       <c r="U9">
         <f t="shared" si="11"/>
-        <v>53.4375</v>
+        <v>47.8125</v>
       </c>
       <c r="V9">
         <f t="shared" si="12"/>
@@ -18104,32 +18121,37 @@
         <f t="shared" si="3"/>
         <v>6.25E-2</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1">
         <v>4</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AC9" s="1">
         <f t="shared" si="13"/>
-        <v>540</v>
-      </c>
-      <c r="AC9" s="1">
-        <f>AC8+IF($AB$2&gt;AE8,-_xlfn.BITRSHIFT(AB8,AA8),_xlfn.BITRSHIFT(AB8,AA8))</f>
-        <v>540</v>
-      </c>
-      <c r="AD9">
+        <v>2592</v>
+      </c>
+      <c r="AD9" s="1">
         <f t="shared" si="14"/>
-        <v>-720</v>
+        <v>2144</v>
       </c>
       <c r="AE9">
         <f t="shared" si="15"/>
-        <v>12240</v>
+        <v>720</v>
       </c>
       <c r="AF9">
+        <f t="shared" si="16"/>
+        <v>10800</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="17"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="AH9">
         <f t="shared" si="4"/>
-        <v>4.90059381963448E-16</v>
-      </c>
-      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>6.25E-2</v>
       </c>
       <c r="AM9">
         <v>1594</v>
@@ -18172,11 +18194,11 @@
       </c>
       <c r="R10" s="1">
         <f t="shared" si="8"/>
-        <v>247.75</v>
+        <v>2306</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="9"/>
-        <v>340.75</v>
+        <v>2458</v>
       </c>
       <c r="T10">
         <f t="shared" si="10"/>
@@ -18184,7 +18206,7 @@
       </c>
       <c r="U10">
         <f t="shared" si="11"/>
-        <v>54.84375</v>
+        <v>49.21875</v>
       </c>
       <c r="V10">
         <f t="shared" si="12"/>
@@ -18198,32 +18220,40 @@
         <f t="shared" si="3"/>
         <v>3.125E-2</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1">
         <v>5</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AC10" s="1">
         <f t="shared" si="13"/>
-        <v>507</v>
-      </c>
-      <c r="AC10" s="1">
-        <f>AC9+IF($AB$2&gt;AE9,-_xlfn.BITRSHIFT(AB9,AA9),_xlfn.BITRSHIFT(AB9,AA9))</f>
-        <v>507</v>
-      </c>
-      <c r="AD10">
+        <v>2458</v>
+      </c>
+      <c r="AD10" s="1">
         <f t="shared" si="14"/>
-        <v>360</v>
+        <v>2306</v>
       </c>
       <c r="AE10">
         <f t="shared" si="15"/>
-        <v>12600</v>
+        <v>360</v>
       </c>
       <c r="AF10">
+        <f t="shared" si="16"/>
+        <v>11160</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="17"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="AH10">
         <f t="shared" si="4"/>
-        <v>-2.45029690981724E-16</v>
-      </c>
-      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="AM10">
+        <v>10346</v>
       </c>
     </row>
     <row r="11" spans="7:44" x14ac:dyDescent="0.25">
@@ -18243,38 +18273,71 @@
         <v>6</v>
       </c>
       <c r="R11" s="1">
-        <f t="shared" ref="R11:R17" si="16">R10+IF(T10&gt;0,-S10*V10,S10*V10)</f>
-        <v>237.1015625</v>
+        <f t="shared" ref="R11:R17" si="18">R10+IF(T10&gt;0,-S10*V10,S10*V10)</f>
+        <v>2229.1875</v>
       </c>
       <c r="S11" s="1">
-        <f t="shared" ref="S11:S17" si="17">S10+IF(T10&gt;0,R10*V10,-R10*V10)</f>
-        <v>348.4921875</v>
+        <f t="shared" ref="S11:S17" si="19">S10+IF(T10&gt;0,R10*V10,-R10*V10)</f>
+        <v>2530.0625</v>
       </c>
       <c r="T11">
-        <f t="shared" ref="T11:T17" si="18">IF($R$2&gt;U10,ABS(T10/2),-ABS(T10/2))</f>
+        <f t="shared" ref="T11:T17" si="20">IF($R$2&gt;U10,ABS(T10/2),-ABS(T10/2))</f>
         <v>0.703125</v>
       </c>
       <c r="U11">
-        <f t="shared" ref="U11:U17" si="19">T11+U10</f>
-        <v>55.546875</v>
+        <f t="shared" ref="U11:U17" si="21">T11+U10</f>
+        <v>49.921875</v>
       </c>
       <c r="V11">
-        <f t="shared" ref="V11:V17" si="20">2^-Q11</f>
+        <f t="shared" ref="V11:V17" si="22">2^-Q11</f>
         <v>1.5625E-2</v>
       </c>
       <c r="W11">
-        <f t="shared" ref="W11:W17" si="21">COS(RADIANS(T11))</f>
+        <f t="shared" ref="W11:W17" si="23">COS(RADIANS(T11))</f>
         <v>0.9999247018391445</v>
       </c>
       <c r="X11">
-        <f t="shared" ref="X11:X17" si="22">2^-Q11</f>
+        <f t="shared" ref="X11:X17" si="24">2^-Q11</f>
         <v>1.5625E-2</v>
       </c>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11">
-        <f>SUM(AD5:AD10)</f>
-        <v>12600</v>
+      <c r="AB11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC11" s="1">
+        <f t="shared" si="13"/>
+        <v>2386</v>
+      </c>
+      <c r="AD11" s="1">
+        <f t="shared" si="14"/>
+        <v>2382</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="15"/>
+        <v>180</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="16"/>
+        <v>11340</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="17"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="AI11">
+        <f t="shared" si="5"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AL11">
+        <f>AM11*AM10</f>
+        <v>40.4140625</v>
+      </c>
+      <c r="AM11">
+        <f>90/23040</f>
+        <v>3.90625E-3</v>
       </c>
     </row>
     <row r="12" spans="7:44" x14ac:dyDescent="0.25">
@@ -18290,34 +18353,64 @@
         <v>7</v>
       </c>
       <c r="R12" s="1">
-        <f t="shared" si="16"/>
-        <v>231.6563720703125</v>
+        <f t="shared" si="18"/>
+        <v>2189.6552734375</v>
       </c>
       <c r="S12" s="1">
-        <f t="shared" si="17"/>
-        <v>352.1968994140625</v>
+        <f t="shared" si="19"/>
+        <v>2564.8935546875</v>
       </c>
       <c r="T12">
-        <f t="shared" si="18"/>
-        <v>-0.3515625</v>
+        <f t="shared" si="20"/>
+        <v>0.3515625</v>
       </c>
       <c r="U12">
-        <f t="shared" si="19"/>
-        <v>55.1953125</v>
+        <f t="shared" si="21"/>
+        <v>50.2734375</v>
       </c>
       <c r="V12">
-        <f t="shared" si="20"/>
-        <v>7.8125E-3</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="21"/>
-        <v>0.99998117528260111</v>
-      </c>
-      <c r="X12">
         <f t="shared" si="22"/>
         <v>7.8125E-3</v>
       </c>
-      <c r="AB12" s="1"/>
+      <c r="W12">
+        <f t="shared" si="23"/>
+        <v>0.99998117528260111</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="24"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC12" s="1">
+        <f t="shared" si="13"/>
+        <v>2349</v>
+      </c>
+      <c r="AD12" s="1">
+        <f t="shared" si="14"/>
+        <v>2419</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="15"/>
+        <v>90</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="16"/>
+        <v>11430</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="17"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="4"/>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="5"/>
+        <v>7.8125E-3</v>
+      </c>
       <c r="AK12">
         <f>1594^2</f>
         <v>2540836</v>
@@ -18332,31 +18425,62 @@
         <v>8</v>
       </c>
       <c r="R13" s="1">
+        <f t="shared" si="18"/>
+        <v>2169.6170425415039</v>
+      </c>
+      <c r="S13" s="1">
+        <f t="shared" si="19"/>
+        <v>2582.0002365112305</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="20"/>
+        <v>-0.17578125</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="21"/>
+        <v>50.09765625</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="22"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="23"/>
+        <v>0.99999529380957619</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="24"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC13" s="1">
+        <f t="shared" si="13"/>
+        <v>2331</v>
+      </c>
+      <c r="AD13" s="1">
+        <f t="shared" si="14"/>
+        <v>2437</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="15"/>
+        <v>45</v>
+      </c>
+      <c r="AF13">
         <f t="shared" si="16"/>
-        <v>234.40791034698486</v>
-      </c>
-      <c r="S13" s="1">
+        <v>11475</v>
+      </c>
+      <c r="AG13">
         <f t="shared" si="17"/>
-        <v>350.38708400726318</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="18"/>
-        <v>-0.17578125</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="19"/>
-        <v>55.01953125</v>
-      </c>
-      <c r="V13">
-        <f t="shared" si="20"/>
         <v>3.90625E-3</v>
       </c>
-      <c r="W13">
-        <f t="shared" si="21"/>
-        <v>0.99999529380957619</v>
-      </c>
-      <c r="X13">
-        <f t="shared" si="22"/>
+      <c r="AH13">
+        <f t="shared" si="4"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="AI13">
+        <f t="shared" si="5"/>
         <v>3.90625E-3</v>
       </c>
       <c r="AK13">
@@ -18369,31 +18493,62 @@
         <v>9</v>
       </c>
       <c r="R14" s="1">
+        <f t="shared" si="18"/>
+        <v>2179.7029809653759</v>
+      </c>
+      <c r="S14" s="1">
+        <f t="shared" si="19"/>
+        <v>2573.5251699388027</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="20"/>
+        <v>-8.7890625E-2</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="21"/>
+        <v>50.009765625</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="22"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="23"/>
+        <v>0.99999882345170188</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="24"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>9</v>
+      </c>
+      <c r="AC14" s="1">
+        <f t="shared" si="13"/>
+        <v>2322</v>
+      </c>
+      <c r="AD14" s="1">
+        <f t="shared" si="14"/>
+        <v>2446</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="15"/>
+        <v>22.5</v>
+      </c>
+      <c r="AF14">
         <f t="shared" si="16"/>
-        <v>235.77660989388824</v>
-      </c>
-      <c r="S14" s="1">
+        <v>11497.5</v>
+      </c>
+      <c r="AG14">
         <f t="shared" si="17"/>
-        <v>349.47142810747027</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="18"/>
-        <v>-8.7890625E-2</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="19"/>
-        <v>54.931640625</v>
-      </c>
-      <c r="V14">
-        <f t="shared" si="20"/>
         <v>1.953125E-3</v>
       </c>
-      <c r="W14">
-        <f t="shared" si="21"/>
-        <v>0.99999882345170188</v>
-      </c>
-      <c r="X14">
-        <f t="shared" si="22"/>
+      <c r="AH14">
+        <f t="shared" si="4"/>
+        <v>0.92387953251128674</v>
+      </c>
+      <c r="AI14">
+        <f t="shared" si="5"/>
         <v>1.953125E-3</v>
       </c>
       <c r="AK14">
@@ -18406,50 +18561,63 @@
         <v>10</v>
       </c>
       <c r="R15" s="1">
-        <f t="shared" si="16"/>
-        <v>236.45917127691064</v>
+        <f t="shared" si="18"/>
+        <v>2184.7293973129126</v>
       </c>
       <c r="S15" s="1">
-        <f t="shared" si="17"/>
-        <v>349.01092691627127</v>
+        <f t="shared" si="19"/>
+        <v>2569.2679375541047</v>
       </c>
       <c r="T15">
-        <f t="shared" si="18"/>
-        <v>4.39453125E-2</v>
+        <f t="shared" si="20"/>
+        <v>-4.39453125E-2</v>
       </c>
       <c r="U15">
-        <f t="shared" si="19"/>
-        <v>54.9755859375</v>
+        <f t="shared" si="21"/>
+        <v>49.9658203125</v>
       </c>
       <c r="V15">
-        <f t="shared" si="20"/>
-        <v>9.765625E-4</v>
-      </c>
-      <c r="W15">
-        <f t="shared" si="21"/>
-        <v>0.99999970586288223</v>
-      </c>
-      <c r="X15">
         <f t="shared" si="22"/>
         <v>9.765625E-4</v>
       </c>
-      <c r="AB15">
-        <v>1</v>
-      </c>
-      <c r="AC15">
-        <v>0</v>
+      <c r="W15">
+        <f t="shared" si="23"/>
+        <v>0.99999970586288223</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="24"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC15" s="1">
+        <f t="shared" si="13"/>
+        <v>2318</v>
+      </c>
+      <c r="AD15" s="1">
+        <f t="shared" si="14"/>
+        <v>2450</v>
       </c>
       <c r="AE15">
-        <v>1</v>
+        <f t="shared" si="15"/>
+        <v>11.25</v>
       </c>
       <c r="AF15">
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>11508.75</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="17"/>
+        <v>9.765625E-4</v>
       </c>
       <c r="AH15">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0.98078528040323043</v>
       </c>
       <c r="AI15">
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>9.765625E-4</v>
       </c>
     </row>
     <row r="16" spans="7:44" x14ac:dyDescent="0.25">
@@ -18457,53 +18625,66 @@
         <v>11</v>
       </c>
       <c r="R16" s="1">
-        <f t="shared" si="16"/>
-        <v>236.11834029359397</v>
+        <f t="shared" si="18"/>
+        <v>2187.2384480331802</v>
       </c>
       <c r="S16" s="1">
-        <f t="shared" si="17"/>
-        <v>349.24184407572136</v>
+        <f t="shared" si="19"/>
+        <v>2567.1344127520415</v>
       </c>
       <c r="T16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2.197265625E-2</v>
       </c>
       <c r="U16">
-        <f t="shared" si="19"/>
-        <v>54.99755859375</v>
+        <f t="shared" si="21"/>
+        <v>49.98779296875</v>
       </c>
       <c r="V16">
-        <f t="shared" si="20"/>
-        <v>4.8828125E-4</v>
-      </c>
-      <c r="W16">
-        <f t="shared" si="21"/>
-        <v>0.99999992646571789</v>
-      </c>
-      <c r="X16">
         <f t="shared" si="22"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="AB16">
-        <v>1</v>
-      </c>
-      <c r="AC16">
-        <v>11520</v>
+      <c r="W16">
+        <f t="shared" si="23"/>
+        <v>0.99999992646571789</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="24"/>
+        <v>4.8828125E-4</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>11</v>
+      </c>
+      <c r="AC16" s="1">
+        <f t="shared" si="13"/>
+        <v>2316</v>
+      </c>
+      <c r="AD16" s="1">
+        <f t="shared" si="14"/>
+        <v>2452</v>
       </c>
       <c r="AE16">
-        <v>1</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>23</v>
+        <f t="shared" si="15"/>
+        <v>5.625</v>
+      </c>
+      <c r="AF16">
+        <f t="shared" si="16"/>
+        <v>11514.375</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" si="17"/>
+        <v>4.8828125E-4</v>
       </c>
       <c r="AH16">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>0.99518472667219693</v>
       </c>
       <c r="AI16">
-        <v>115200</v>
-      </c>
-    </row>
-    <row r="17" spans="8:35" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>4.8828125E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="8:37" x14ac:dyDescent="0.25">
       <c r="H17" s="1">
         <v>142</v>
       </c>
@@ -18514,53 +18695,66 @@
         <v>12</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" si="16"/>
-        <v>235.94781204941637</v>
+        <f t="shared" si="18"/>
+        <v>2185.9849644332035</v>
       </c>
       <c r="S17" s="1">
-        <f t="shared" si="17"/>
-        <v>349.35713623406787</v>
+        <f t="shared" si="19"/>
+        <v>2568.2024002754952</v>
       </c>
       <c r="T17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.0986328125E-2</v>
       </c>
       <c r="U17">
-        <f t="shared" si="19"/>
-        <v>55.008544921875</v>
+        <f t="shared" si="21"/>
+        <v>49.998779296875</v>
       </c>
       <c r="V17">
-        <f t="shared" si="20"/>
-        <v>2.44140625E-4</v>
-      </c>
-      <c r="W17">
-        <f t="shared" si="21"/>
-        <v>0.99999998161642933</v>
-      </c>
-      <c r="X17">
         <f t="shared" si="22"/>
         <v>2.44140625E-4</v>
       </c>
-      <c r="AB17">
-        <v>-66355199</v>
-      </c>
-      <c r="AC17">
-        <v>17280</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>22</v>
+      <c r="W17">
+        <f t="shared" si="23"/>
+        <v>0.99999998161642933</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="24"/>
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC17" s="1">
+        <f t="shared" si="13"/>
+        <v>2315</v>
+      </c>
+      <c r="AD17" s="1">
+        <f t="shared" si="14"/>
+        <v>2453</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="15"/>
+        <v>2.8125</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" si="16"/>
+        <v>11517.1875</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" si="17"/>
+        <v>2.44140625E-4</v>
       </c>
       <c r="AH17">
-        <v>-32767</v>
+        <f t="shared" si="4"/>
+        <v>0.99879545620517241</v>
       </c>
       <c r="AI17">
-        <v>17280</v>
-      </c>
-    </row>
-    <row r="18" spans="8:35" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.44140625E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="8:37" x14ac:dyDescent="0.25">
       <c r="H18" s="1">
         <f>H17^2</f>
         <v>20164</v>
@@ -18573,53 +18767,66 @@
         <v>13</v>
       </c>
       <c r="R18" s="1">
-        <f t="shared" ref="R18:R20" si="23">R17+IF(T17&gt;0,-S17*V17,S17*V17)</f>
-        <v>235.86251977982798</v>
+        <f t="shared" ref="R18:R20" si="25">R17+IF(T17&gt;0,-S17*V17,S17*V17)</f>
+        <v>2185.3579618940739</v>
       </c>
       <c r="S18" s="1">
-        <f t="shared" ref="S18:S20" si="24">S17+IF(T17&gt;0,R17*V17,-R17*V17)</f>
-        <v>349.41474068036899</v>
+        <f t="shared" ref="S18:S20" si="26">S17+IF(T17&gt;0,R17*V17,-R17*V17)</f>
+        <v>2568.7360880109527</v>
       </c>
       <c r="T18">
-        <f t="shared" ref="T18:T20" si="25">IF($R$2&gt;U17,ABS(T17/2),-ABS(T17/2))</f>
-        <v>-5.4931640625E-3</v>
+        <f t="shared" ref="T18:T20" si="27">IF($R$2&gt;U17,ABS(T17/2),-ABS(T17/2))</f>
+        <v>5.4931640625E-3</v>
       </c>
       <c r="U18">
-        <f t="shared" ref="U18:U20" si="26">T18+U17</f>
-        <v>55.0030517578125</v>
+        <f t="shared" ref="U18:U20" si="28">T18+U17</f>
+        <v>50.0042724609375</v>
       </c>
       <c r="V18">
-        <f t="shared" ref="V18:V20" si="27">2^-Q18</f>
+        <f t="shared" ref="V18:V20" si="29">2^-Q18</f>
         <v>1.220703125E-4</v>
       </c>
       <c r="W18">
-        <f t="shared" ref="W18:W21" si="28">COS(RADIANS(T18))</f>
+        <f t="shared" ref="W18:W21" si="30">COS(RADIANS(T18))</f>
         <v>0.99999999540410733</v>
       </c>
       <c r="X18">
-        <f t="shared" ref="X18:X20" si="29">2^-Q18</f>
+        <f t="shared" ref="X18:X20" si="31">2^-Q18</f>
         <v>1.220703125E-4</v>
       </c>
-      <c r="AB18">
-        <v>-16588799</v>
-      </c>
-      <c r="AC18">
-        <v>191102990400</v>
-      </c>
-      <c r="AE18" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>25</v>
+      <c r="AB18" s="1">
+        <v>13</v>
+      </c>
+      <c r="AC18" s="1">
+        <f t="shared" si="13"/>
+        <v>2315</v>
+      </c>
+      <c r="AD18" s="1">
+        <f t="shared" si="14"/>
+        <v>2453</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="15"/>
+        <v>1.40625</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="16"/>
+        <v>11518.59375</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" si="17"/>
+        <v>1.220703125E-4</v>
       </c>
       <c r="AH18">
-        <v>-8191</v>
+        <f t="shared" si="4"/>
+        <v>0.99969881869620425</v>
       </c>
       <c r="AI18">
-        <v>14400</v>
-      </c>
-    </row>
-    <row r="19" spans="8:35" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>1.220703125E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="8:37" x14ac:dyDescent="0.25">
       <c r="H19" s="1">
         <f>SQRT(H18+I18)</f>
         <v>254.33245958783948</v>
@@ -18628,161 +18835,837 @@
         <v>14</v>
       </c>
       <c r="R19" s="1">
-        <f t="shared" si="23"/>
-        <v>235.90517294641495</v>
+        <f t="shared" si="25"/>
+        <v>2185.0443954770803</v>
       </c>
       <c r="S19" s="1">
-        <f t="shared" si="24"/>
-        <v>349.38594886887245</v>
+        <f t="shared" si="26"/>
+        <v>2569.0028553402854</v>
       </c>
       <c r="T19">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>-2.74658203125E-3</v>
       </c>
       <c r="U19">
-        <f t="shared" si="26"/>
-        <v>55.00030517578125</v>
+        <f t="shared" si="28"/>
+        <v>50.00152587890625</v>
       </c>
       <c r="V19">
-        <f t="shared" si="27"/>
-        <v>6.103515625E-5</v>
-      </c>
-      <c r="W19">
-        <f t="shared" si="28"/>
-        <v>0.99999999885102686</v>
-      </c>
-      <c r="X19">
         <f t="shared" si="29"/>
         <v>6.103515625E-5</v>
       </c>
-      <c r="AB19">
-        <v>275188289587201</v>
-      </c>
-      <c r="AC19">
-        <v>214990860960</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>27</v>
+      <c r="W19">
+        <f t="shared" si="30"/>
+        <v>0.99999999885102686</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="31"/>
+        <v>6.103515625E-5</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>14</v>
+      </c>
+      <c r="AC19" s="1">
+        <f t="shared" si="13"/>
+        <v>2315</v>
+      </c>
+      <c r="AD19" s="1">
+        <f t="shared" si="14"/>
+        <v>2453</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" si="15"/>
+        <v>0.703125</v>
+      </c>
+      <c r="AF19">
+        <f t="shared" si="16"/>
+        <v>11519.296875</v>
+      </c>
+      <c r="AG19">
+        <f t="shared" si="17"/>
+        <v>6.103515625E-5</v>
       </c>
       <c r="AH19">
-        <v>18433</v>
+        <f t="shared" si="4"/>
+        <v>0.9999247018391445</v>
       </c>
       <c r="AI19">
-        <v>12960</v>
-      </c>
-    </row>
-    <row r="20" spans="8:35" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>6.103515625E-5</v>
+      </c>
+      <c r="AK19">
+        <f>ATAN2(1500,1300)</f>
+        <v>0.71409069861215801</v>
+      </c>
+    </row>
+    <row r="20" spans="8:37" x14ac:dyDescent="0.25">
       <c r="Q20" s="1">
         <v>15</v>
       </c>
       <c r="R20" s="1">
-        <f t="shared" si="23"/>
-        <v>235.92649777239572</v>
+        <f t="shared" si="25"/>
+        <v>2185.2011949677626</v>
       </c>
       <c r="S20" s="1">
-        <f t="shared" si="24"/>
-        <v>349.37155035978145</v>
+        <f t="shared" si="26"/>
+        <v>2568.8694908141943</v>
       </c>
       <c r="T20">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>-1.373291015625E-3</v>
       </c>
       <c r="U20">
-        <f t="shared" si="26"/>
-        <v>54.998931884765625</v>
+        <f t="shared" si="28"/>
+        <v>50.000152587890625</v>
       </c>
       <c r="V20">
-        <f t="shared" si="27"/>
-        <v>3.0517578125E-5</v>
-      </c>
-      <c r="W20">
-        <f t="shared" si="28"/>
-        <v>0.99999999971275666</v>
-      </c>
-      <c r="X20">
         <f t="shared" si="29"/>
         <v>3.0517578125E-5</v>
       </c>
-      <c r="AB20">
-        <v>429981709478401</v>
-      </c>
-      <c r="AC20">
-        <v>-1.9813535351192374E+17</v>
-      </c>
-    </row>
-    <row r="21" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="W20">
+        <f t="shared" si="30"/>
+        <v>0.99999999971275666</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="31"/>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>15</v>
+      </c>
+      <c r="AC20" s="1">
+        <f t="shared" si="13"/>
+        <v>2315</v>
+      </c>
+      <c r="AD20" s="1">
+        <f t="shared" si="14"/>
+        <v>2453</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="15"/>
+        <v>0.3515625</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="16"/>
+        <v>11519.6484375</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" si="17"/>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="4"/>
+        <v>0.99998117528260111</v>
+      </c>
+      <c r="AI20">
+        <f t="shared" si="5"/>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="AK20">
+        <f>DEGREES(AK19)</f>
+        <v>40.91438322002513</v>
+      </c>
+    </row>
+    <row r="21" spans="8:37" x14ac:dyDescent="0.25">
       <c r="R21" s="1">
         <f>R20*T21</f>
-        <v>36568.607154721336</v>
+        <v>338706.18522000319</v>
       </c>
       <c r="S21" s="1">
         <f>S20*T21</f>
-        <v>54152.590305766127</v>
+        <v>398174.77107620012</v>
       </c>
       <c r="T21">
         <v>155</v>
       </c>
       <c r="W21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>-0.90630778703664994</v>
       </c>
-      <c r="AB21">
-        <v>7.132915724600202E+19</v>
-      </c>
-      <c r="AC21">
-        <v>-4.3341938099699392E+16</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="8:35" x14ac:dyDescent="0.25">
+      <c r="AC21" s="1">
+        <f>AC20*AE21</f>
+        <v>358825</v>
+      </c>
+      <c r="AD21" s="1">
+        <f>AD20*AE21</f>
+        <v>380215</v>
+      </c>
+      <c r="AE21">
+        <v>155</v>
+      </c>
+      <c r="AH21">
+        <f t="shared" si="4"/>
+        <v>-0.90630778703664994</v>
+      </c>
+    </row>
+    <row r="22" spans="8:37" x14ac:dyDescent="0.25">
       <c r="R22" s="1">
         <f>ROUND(R21,0)</f>
-        <v>36569</v>
+        <v>338706</v>
       </c>
       <c r="S22" s="1">
         <f>ROUND(S21,0)</f>
-        <v>54153</v>
-      </c>
-    </row>
-    <row r="23" spans="8:35" x14ac:dyDescent="0.25">
+        <v>398175</v>
+      </c>
+      <c r="AC22" s="1">
+        <f>ROUND(AC21,0)</f>
+        <v>358825</v>
+      </c>
+      <c r="AD22" s="1">
+        <f>ROUND(AD21,0)</f>
+        <v>380215</v>
+      </c>
+    </row>
+    <row r="23" spans="8:37" x14ac:dyDescent="0.25">
       <c r="R23" s="1">
         <f>_xlfn.BITRSHIFT(R22,8)</f>
-        <v>142</v>
+        <v>1323</v>
       </c>
       <c r="S23" s="1">
         <f>_xlfn.BITRSHIFT(S22,8)</f>
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="8:35" x14ac:dyDescent="0.25">
+        <v>1555</v>
+      </c>
+      <c r="AC23" s="1">
+        <f>_xlfn.BITRSHIFT(AC22,8)</f>
+        <v>1401</v>
+      </c>
+      <c r="AD23" s="1">
+        <f>_xlfn.BITRSHIFT(AD22,8)</f>
+        <v>1485</v>
+      </c>
+      <c r="AE23">
+        <f>AC3*2048</f>
+        <v>1448.1546878700494</v>
+      </c>
+    </row>
+    <row r="24" spans="8:37" x14ac:dyDescent="0.25">
       <c r="R24" s="1">
         <f>R23^2</f>
-        <v>20164</v>
+        <v>1750329</v>
       </c>
       <c r="S24" s="1">
         <f>S23^2</f>
-        <v>44521</v>
-      </c>
-    </row>
-    <row r="25" spans="8:35" x14ac:dyDescent="0.25">
+        <v>2418025</v>
+      </c>
+      <c r="AC24" s="1">
+        <f>AC23^2</f>
+        <v>1962801</v>
+      </c>
+      <c r="AD24" s="1">
+        <f>AD23^2</f>
+        <v>2205225</v>
+      </c>
+    </row>
+    <row r="25" spans="8:37" x14ac:dyDescent="0.25">
       <c r="R25" s="1">
         <f>SQRT(R24+S24)</f>
-        <v>254.33245958783948</v>
+        <v>2041.6547210534891</v>
+      </c>
+      <c r="AC25" s="1">
+        <f>SQRT(AC24+AD24)</f>
+        <v>2041.5743924726328</v>
+      </c>
+    </row>
+    <row r="26" spans="8:37" x14ac:dyDescent="0.25">
+      <c r="AC26" s="1">
+        <f>AC20*128</f>
+        <v>296320</v>
+      </c>
+      <c r="AD26" s="1">
+        <f>AD20*128</f>
+        <v>313984</v>
+      </c>
+    </row>
+    <row r="28" spans="8:37" x14ac:dyDescent="0.25">
+      <c r="AE28">
+        <v>9</v>
+      </c>
+      <c r="AF28">
+        <f>AE28*256</f>
+        <v>2304</v>
+      </c>
+      <c r="AG28">
+        <f>AE28*4096</f>
+        <v>36864</v>
+      </c>
+    </row>
+    <row r="29" spans="8:37" x14ac:dyDescent="0.25">
+      <c r="AB29">
+        <f>1500^2+1300^2</f>
+        <v>3940000</v>
+      </c>
+      <c r="AE29">
+        <v>20</v>
+      </c>
+      <c r="AF29">
+        <f>AE29*256</f>
+        <v>5120</v>
+      </c>
+      <c r="AG29">
+        <f>AE29*4096</f>
+        <v>81920</v>
+      </c>
+    </row>
+    <row r="30" spans="8:37" x14ac:dyDescent="0.25">
+      <c r="AB30">
+        <f>SQRT(AB29)</f>
+        <v>1984.9433241279207</v>
+      </c>
+      <c r="AE30">
+        <f>ATAN2(AE28,AE29)</f>
+        <v>1.1479424006619559</v>
+      </c>
+      <c r="AF30">
+        <f>ATAN2(AF28,AF29)</f>
+        <v>1.1479424006619559</v>
+      </c>
+      <c r="AG30">
+        <f>ATAN2(AG28,AG29)</f>
+        <v>1.1479424006619559</v>
+      </c>
+    </row>
+    <row r="31" spans="8:37" x14ac:dyDescent="0.25">
+      <c r="AB31">
+        <f>3269*155</f>
+        <v>506695</v>
+      </c>
+      <c r="AE31">
+        <f>DEGREES(AE30)</f>
+        <v>65.772254682045826</v>
+      </c>
+      <c r="AF31">
+        <f>DEGREES(AF30)</f>
+        <v>65.772254682045826</v>
+      </c>
+      <c r="AG31">
+        <f>DEGREES(AG30)</f>
+        <v>65.772254682045826</v>
+      </c>
+    </row>
+    <row r="32" spans="8:37" x14ac:dyDescent="0.25">
+      <c r="AB32">
+        <f>_xlfn.BITRSHIFT(AB31,8)</f>
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="36" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC36" s="4"/>
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="4"/>
+      <c r="AF36" s="4"/>
+      <c r="AG36" s="4"/>
+      <c r="AH36" s="4"/>
+    </row>
+    <row r="37" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB37" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC37" s="1">
+        <v>10346</v>
+      </c>
+    </row>
+    <row r="38" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AC38" s="1">
+        <f>COS(RADIANS(AC37))</f>
+        <v>-6.9756473744129771E-2</v>
+      </c>
+      <c r="AD38" s="1">
+        <f>SIN(RADIANS(AC37))</f>
+        <v>-0.99756405025982398</v>
+      </c>
+    </row>
+    <row r="39" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG39" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="1">
+        <v>1542</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>1337</v>
+      </c>
+      <c r="AE40">
+        <v>11520</v>
+      </c>
+      <c r="AF40" s="1">
+        <v>11520</v>
+      </c>
+      <c r="AG40">
+        <f>2^AB40</f>
+        <v>1</v>
+      </c>
+      <c r="AH40">
+        <f t="shared" ref="AH40:AH55" si="32">COS(RADIANS(AE40))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC41" s="1">
+        <f t="shared" ref="AC41:AC55" si="33">AC40+IF(AD40&gt;0,(AD40*2^(-AB40)),-(AD40*2^(-AB40)))</f>
+        <v>2879</v>
+      </c>
+      <c r="AD41" s="1">
+        <f t="shared" ref="AD41:AD55" si="34">AD40+IF(AD40&gt;0,-(AC40*2^(-AB40)),(AC40*2^(-AB40)))</f>
+        <v>-205</v>
+      </c>
+      <c r="AE41">
+        <f t="shared" ref="AE41:AE55" si="35">IF(AD41&gt;0,ABS(AE40/2),-ABS(AE40/2))</f>
+        <v>-5760</v>
+      </c>
+      <c r="AF41">
+        <f>AE41+AF40</f>
+        <v>5760</v>
+      </c>
+      <c r="AG41">
+        <f t="shared" ref="AG41:AG55" si="36">2^-AB41</f>
+        <v>0.5</v>
+      </c>
+      <c r="AH41">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB42" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC42" s="1">
+        <f t="shared" si="33"/>
+        <v>2981.5</v>
+      </c>
+      <c r="AD42" s="1">
+        <f t="shared" si="34"/>
+        <v>1234.5</v>
+      </c>
+      <c r="AE42">
+        <f>IF(AD42&gt;0,ABS(AE41/2),-ABS(AE41/2))</f>
+        <v>2880</v>
+      </c>
+      <c r="AF42">
+        <f>AE42+AF41</f>
+        <v>8640</v>
+      </c>
+      <c r="AG42">
+        <f t="shared" si="36"/>
+        <v>0.25</v>
+      </c>
+      <c r="AH42">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB43" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC43" s="1">
+        <f t="shared" si="33"/>
+        <v>3290.125</v>
+      </c>
+      <c r="AD43" s="1">
+        <f t="shared" si="34"/>
+        <v>489.125</v>
+      </c>
+      <c r="AE43">
+        <f t="shared" si="35"/>
+        <v>1440</v>
+      </c>
+      <c r="AF43">
+        <f t="shared" ref="AF41:AF55" si="37">AE43+AF42</f>
+        <v>10080</v>
+      </c>
+      <c r="AG43">
+        <f t="shared" si="36"/>
+        <v>0.125</v>
+      </c>
+      <c r="AH43">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB44" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC44" s="1">
+        <f t="shared" si="33"/>
+        <v>3351.265625</v>
+      </c>
+      <c r="AD44" s="1">
+        <f t="shared" si="34"/>
+        <v>77.859375</v>
+      </c>
+      <c r="AE44">
+        <f t="shared" si="35"/>
+        <v>720</v>
+      </c>
+      <c r="AF44">
+        <f t="shared" si="37"/>
+        <v>10800</v>
+      </c>
+      <c r="AG44">
+        <f t="shared" si="36"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="AH44">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB45" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC45" s="1">
+        <f t="shared" si="33"/>
+        <v>3356.1318359375</v>
+      </c>
+      <c r="AD45" s="1">
+        <f t="shared" si="34"/>
+        <v>-131.5947265625</v>
+      </c>
+      <c r="AE45">
+        <f t="shared" si="35"/>
+        <v>-360</v>
+      </c>
+      <c r="AF45">
+        <f t="shared" si="37"/>
+        <v>10440</v>
+      </c>
+      <c r="AG45">
+        <f t="shared" si="36"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="AH45">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB46" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC46" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.2441711425781</v>
+      </c>
+      <c r="AD46" s="1">
+        <f t="shared" si="34"/>
+        <v>-26.715606689453125</v>
+      </c>
+      <c r="AE46">
+        <f t="shared" si="35"/>
+        <v>-180</v>
+      </c>
+      <c r="AF46">
+        <f t="shared" si="37"/>
+        <v>10260</v>
+      </c>
+      <c r="AG46">
+        <f t="shared" si="36"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AH46">
+        <f t="shared" si="32"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB47" s="1">
+        <v>7</v>
+      </c>
+      <c r="AC47" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.6616024971008</v>
+      </c>
+      <c r="AD47" s="1">
+        <f t="shared" si="34"/>
+        <v>25.788208484649658</v>
+      </c>
+      <c r="AE47">
+        <f t="shared" si="35"/>
+        <v>90</v>
+      </c>
+      <c r="AF47">
+        <f t="shared" si="37"/>
+        <v>10350</v>
+      </c>
+      <c r="AG47">
+        <f t="shared" si="36"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="AH47">
+        <f t="shared" si="32"/>
+        <v>6.1257422745431001E-17</v>
+      </c>
+    </row>
+    <row r="48" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB48" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC48" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.8630728758872</v>
+      </c>
+      <c r="AD48" s="1">
+        <f t="shared" si="34"/>
+        <v>-0.46696028485894203</v>
+      </c>
+      <c r="AE48">
+        <f t="shared" si="35"/>
+        <v>-45</v>
+      </c>
+      <c r="AF48">
+        <f t="shared" si="37"/>
+        <v>10305</v>
+      </c>
+      <c r="AG48">
+        <f t="shared" si="36"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="AH48">
+        <f t="shared" si="32"/>
+        <v>0.70710678118654757</v>
+      </c>
+    </row>
+    <row r="49" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB49" s="1">
+        <v>9</v>
+      </c>
+      <c r="AC49" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.8648969394999</v>
+      </c>
+      <c r="AD49" s="1">
+        <f t="shared" si="34"/>
+        <v>12.661411093562492</v>
+      </c>
+      <c r="AE49">
+        <f t="shared" si="35"/>
+        <v>22.5</v>
+      </c>
+      <c r="AF49">
+        <f t="shared" si="37"/>
+        <v>10327.5</v>
+      </c>
+      <c r="AG49">
+        <f t="shared" si="36"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="AH49">
+        <f t="shared" si="32"/>
+        <v>0.92387953251128674</v>
+      </c>
+    </row>
+    <row r="50" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB50" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC50" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.889626258042</v>
+      </c>
+      <c r="AD50" s="1">
+        <f t="shared" si="34"/>
+        <v>6.0972218417275315</v>
+      </c>
+      <c r="AE50">
+        <f t="shared" si="35"/>
+        <v>11.25</v>
+      </c>
+      <c r="AF50">
+        <f t="shared" si="37"/>
+        <v>10338.75</v>
+      </c>
+      <c r="AG50">
+        <f t="shared" si="36"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="AH50">
+        <f t="shared" si="32"/>
+        <v>0.98078528040323043</v>
+      </c>
+    </row>
+    <row r="51" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB51" s="1">
+        <v>11</v>
+      </c>
+      <c r="AC51" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.8955805762466</v>
+      </c>
+      <c r="AD51" s="1">
+        <f t="shared" si="34"/>
+        <v>2.8151030660849123</v>
+      </c>
+      <c r="AE51">
+        <f t="shared" si="35"/>
+        <v>5.625</v>
+      </c>
+      <c r="AF51">
+        <f t="shared" si="37"/>
+        <v>10344.375</v>
+      </c>
+      <c r="AG51">
+        <f t="shared" si="36"/>
+        <v>4.8828125E-4</v>
+      </c>
+      <c r="AH51">
+        <f t="shared" si="32"/>
+        <v>0.99518472667219693</v>
+      </c>
+    </row>
+    <row r="52" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB52" s="1">
+        <v>12</v>
+      </c>
+      <c r="AC52" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.8969551382907</v>
+      </c>
+      <c r="AD52" s="1">
+        <f t="shared" si="34"/>
+        <v>1.1740407708816669</v>
+      </c>
+      <c r="AE52">
+        <f t="shared" si="35"/>
+        <v>2.8125</v>
+      </c>
+      <c r="AF52">
+        <f t="shared" si="37"/>
+        <v>10347.1875</v>
+      </c>
+      <c r="AG52">
+        <f t="shared" si="36"/>
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="AH52">
+        <f t="shared" si="32"/>
+        <v>0.99879545620517241</v>
+      </c>
+    </row>
+    <row r="53" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB53" s="1">
+        <v>13</v>
+      </c>
+      <c r="AC53" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.8972417693381</v>
+      </c>
+      <c r="AD53" s="1">
+        <f t="shared" si="34"/>
+        <v>0.35350928769360768</v>
+      </c>
+      <c r="AE53">
+        <f t="shared" si="35"/>
+        <v>1.40625</v>
+      </c>
+      <c r="AF53">
+        <f t="shared" si="37"/>
+        <v>10348.59375</v>
+      </c>
+      <c r="AG53">
+        <f t="shared" si="36"/>
+        <v>1.220703125E-4</v>
+      </c>
+      <c r="AH53">
+        <f t="shared" si="32"/>
+        <v>0.99969881869620425</v>
+      </c>
+    </row>
+    <row r="54" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB54" s="1">
+        <v>14</v>
+      </c>
+      <c r="AC54" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.8972849223273</v>
+      </c>
+      <c r="AD54" s="1">
+        <f t="shared" si="34"/>
+        <v>-5.6756488889563472E-2</v>
+      </c>
+      <c r="AE54">
+        <f t="shared" si="35"/>
+        <v>-0.703125</v>
+      </c>
+      <c r="AF54">
+        <f t="shared" si="37"/>
+        <v>10347.890625</v>
+      </c>
+      <c r="AG54">
+        <f t="shared" si="36"/>
+        <v>6.103515625E-5</v>
+      </c>
+      <c r="AH54">
+        <f t="shared" si="32"/>
+        <v>0.9999247018391445</v>
+      </c>
+    </row>
+    <row r="55" spans="28:34" x14ac:dyDescent="0.25">
+      <c r="AB55" s="1">
+        <v>15</v>
+      </c>
+      <c r="AC55" s="1">
+        <f t="shared" si="33"/>
+        <v>3360.8972883864685</v>
+      </c>
+      <c r="AD55" s="1">
+        <f t="shared" si="34"/>
+        <v>0.14837640203587155</v>
+      </c>
+      <c r="AE55">
+        <f t="shared" si="35"/>
+        <v>0.3515625</v>
+      </c>
+      <c r="AF55">
+        <f t="shared" si="37"/>
+        <v>10348.2421875</v>
+      </c>
+      <c r="AG55">
+        <f t="shared" si="36"/>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="AH55">
+        <f t="shared" si="32"/>
+        <v>0.99998117528260111</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="G1:M1"/>
-    <mergeCell ref="AA1:AG1"/>
     <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="AB1:AH1"/>
+    <mergeCell ref="AB36:AH36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>